<commit_message>
-added the first benchmark for the experiments.
- TO DO : make commentaries, edit the JMH tests.
</commit_message>
<xml_diff>
--- a/jmh-result-length-scread.xlsx
+++ b/jmh-result-length-scread.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenge\IdeaProjects\INFO-H417-group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F2F4F92-477D-49DF-87CE-6E5917386DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{87D13D64-E59A-456F-B3E1-9FB51CCA2998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="810" windowWidth="28395" windowHeight="11760"/>
+    <workbookView xWindow="690" yWindow="1170" windowWidth="28395" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="jmh-result-length-scread" sheetId="1" r:id="rId1"/>
@@ -20,45 +20,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Benchmark,"Mode","Threads","Samples","Score","Score Error (99,9%)","Unit","Param: fileName"</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"269,502949","2,726122","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\company_name.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,042850","0,017028","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\company_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"35,155531","0,908809","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\complete_cast.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,044529","0,009562","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\comp_cast_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,063665","0,002226","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\info_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"57,080414","0,948987","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\keyword.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,048218","0,006348","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\kind_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,046677","0,004418","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\link_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"511,200897","8,065819","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\movie_info_idx.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"9,391801","0,103431","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\movie_link.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,041707","0,008794","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\role_type.csv</t>
-  </si>
-  <si>
-    <t>benchmark.LengthBenchmark.singleCharacterReader,"avgt",1,5,"0,091956","0,000786","ms/op",C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\schematext.sql</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Score Error (99,9%)</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Param: fileName</t>
+  </si>
+  <si>
+    <t>benchmark.LengthBenchmark.singleCharacterReader</t>
+  </si>
+  <si>
+    <t>avgt</t>
+  </si>
+  <si>
+    <t>ms/op</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\company_name.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\company_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\complete_cast.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\comp_cast_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\info_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\keyword.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\kind_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\link_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\movie_info_idx.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\movie_link.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\role_type.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\lenge\IdeaProjects\INFO-H417-group4\imdb\schematext.sql</t>
   </si>
 </sst>
 </file>
@@ -899,75 +929,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>269.502949</v>
+      </c>
+      <c r="F2">
+        <v>2.7261220000000002</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>4.2849999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.7028000000000001E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>35.155531000000003</v>
+      </c>
+      <c r="F4">
+        <v>0.90880899999999998</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>4.4528999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>9.5619999999999993E-3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
+      <c r="E6">
+        <v>6.3664999999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>2.2260000000000001E-3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>57.080413999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.94898700000000002</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>4.8217999999999997E-2</v>
+      </c>
+      <c r="F8">
+        <v>6.3480000000000003E-3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4.6677000000000003E-2</v>
+      </c>
+      <c r="F9">
+        <v>4.4180000000000001E-3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>511.200897</v>
+      </c>
+      <c r="F10">
+        <v>8.0658189999999994</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>9.3918009999999992</v>
+      </c>
+      <c r="F11">
+        <v>0.103431</v>
+      </c>
+      <c r="G11" t="s">
         <v>10</v>
       </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>4.1707000000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>8.7939999999999997E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>9.1955999999999996E-2</v>
+      </c>
+      <c r="F13">
+        <v>7.8600000000000002E-4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>